<commit_message>
updates some features to improve the logical usabillity & new features to treat data
</commit_message>
<xml_diff>
--- a/123.xlsx
+++ b/123.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.lourenco\Documents\GitHub\GSDA-310\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77914879-BF69-4143-87AA-F9CB7E421A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE8031F-B6AC-4EA8-B43F-CEE8E7C4F08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,21 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>nome</t>
-  </si>
-  <si>
-    <t>valor</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>lucas</t>
   </si>
   <si>
-    <t>ihsa</t>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>rua Graccho rangel, 553</t>
+  </si>
+  <si>
+    <t>rua expedito sauasuh</t>
+  </si>
+  <si>
+    <t>ENDEREÇO</t>
+  </si>
+  <si>
+    <t>CTPS</t>
+  </si>
+  <si>
+    <t>465468 123/RJ</t>
+  </si>
+  <si>
+    <t>123456 64/RJ</t>
+  </si>
+  <si>
+    <t>09706809700</t>
   </si>
 </sst>
 </file>
@@ -75,9 +96,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,45 +380,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>24000</v>
-      </c>
-      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
         <v>45575</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>10000</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="1">
         <v>45576</v>
+      </c>
+      <c r="C3" s="2">
+        <v>12345678910</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
introduces the initial idea of generate docx
</commit_message>
<xml_diff>
--- a/123.xlsx
+++ b/123.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.lourenco\Documents\GitHub\GSDA-310\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE8031F-B6AC-4EA8-B43F-CEE8E7C4F08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179D3283-15A3-408F-BDF8-03877B8DE966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="1815" windowWidth="22980" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>lucas</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>09706809700</t>
+  </si>
+  <si>
+    <t>HORA</t>
   </si>
 </sst>
 </file>
@@ -96,10 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,69 +384,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>45575</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>45576</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D3" s="2">
         <v>12345678910</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>